<commit_message>
updates to msft, goog
</commit_message>
<xml_diff>
--- a/Competition.xlsx
+++ b/Competition.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0E1869C-7F44-4628-9657-EFF10BD253A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1B643A2-4D63-4952-88BA-B29133C40BC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9915" yWindow="2220" windowWidth="18810" windowHeight="13215" activeTab="1" xr2:uid="{5AC812C1-C6FA-4E05-932F-D1EBD613AE9A}"/>
+    <workbookView xWindow="8655" yWindow="0" windowWidth="20145" windowHeight="15465" activeTab="1" xr2:uid="{5AC812C1-C6FA-4E05-932F-D1EBD613AE9A}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="621" uniqueCount="222">
   <si>
     <t>Date</t>
   </si>
@@ -657,6 +657,69 @@
   </si>
   <si>
     <t>2022-07-25, 14:17:17</t>
+  </si>
+  <si>
+    <t>2022-07-26, 09:30:58</t>
+  </si>
+  <si>
+    <t>2022-07-26, 13:50:44</t>
+  </si>
+  <si>
+    <t>SHOP</t>
+  </si>
+  <si>
+    <t>2022-07-26, 09:36:54</t>
+  </si>
+  <si>
+    <t>2022-07-26, 09:38:07</t>
+  </si>
+  <si>
+    <t>2022-07-26, 13:22:20</t>
+  </si>
+  <si>
+    <t>2022-07-26, 13:49:34</t>
+  </si>
+  <si>
+    <t>Total SHOP</t>
+  </si>
+  <si>
+    <t>2022-07-26, 09:55:17</t>
+  </si>
+  <si>
+    <t>2022-07-26, 10:02:10</t>
+  </si>
+  <si>
+    <t>2022-07-26, 10:05:43</t>
+  </si>
+  <si>
+    <t>2022-07-26, 13:50:51</t>
+  </si>
+  <si>
+    <t>2022-07-26, 09:51:41</t>
+  </si>
+  <si>
+    <t>2022-07-26, 10:58:28</t>
+  </si>
+  <si>
+    <t>2022-07-26, 11:04:01</t>
+  </si>
+  <si>
+    <t>2022-07-26, 12:14:00</t>
+  </si>
+  <si>
+    <t>2022-07-26, 12:45:32</t>
+  </si>
+  <si>
+    <t>2022-07-26, 09:31:37</t>
+  </si>
+  <si>
+    <t>2022-07-26, 09:38:49</t>
+  </si>
+  <si>
+    <t>2022-07-26, 12:45:40</t>
+  </si>
+  <si>
+    <t>2022-07-26, 13:49:22</t>
   </si>
 </sst>
 </file>
@@ -1040,13 +1103,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FAE940E-6F97-4759-B7C4-CA0B0F24A13F}">
-  <dimension ref="B3:G11"/>
+  <dimension ref="B3:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C11" sqref="C11"/>
+      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1093,7 +1156,7 @@
         <v>50825.7</v>
       </c>
       <c r="D5" s="3">
-        <f>C5-C4</f>
+        <f t="shared" ref="D5:D11" si="0">C5-C4</f>
         <v>564.55999999999767</v>
       </c>
       <c r="E5" s="5">
@@ -1101,11 +1164,11 @@
         <v>564.55999999999767</v>
       </c>
       <c r="F5" s="4">
-        <f>+C5/C4-1</f>
+        <f t="shared" ref="F5:F11" si="1">+C5/C4-1</f>
         <v>1.123253471767649E-2</v>
       </c>
       <c r="G5" s="7">
-        <f>C5/$C$4-1</f>
+        <f t="shared" ref="G5:G11" si="2">C5/$C$4-1</f>
         <v>1.123253471767649E-2</v>
       </c>
     </row>
@@ -1118,19 +1181,19 @@
         <v>52552.24</v>
       </c>
       <c r="D6" s="3">
-        <f>C6-C5</f>
+        <f t="shared" si="0"/>
         <v>1726.5400000000009</v>
       </c>
       <c r="E6" s="5">
-        <f>C6-$C$4</f>
+        <f t="shared" ref="E6:E11" si="3">C6-$C$4</f>
         <v>2291.0999999999985</v>
       </c>
       <c r="F6" s="4">
-        <f>+C6/C5-1</f>
+        <f t="shared" si="1"/>
         <v>3.3969822353651757E-2</v>
       </c>
       <c r="G6" s="7">
-        <f>C6/$C$4-1</f>
+        <f t="shared" si="2"/>
         <v>4.5583924280268917E-2</v>
       </c>
     </row>
@@ -1143,19 +1206,19 @@
         <v>53245.13</v>
       </c>
       <c r="D7" s="3">
-        <f>C7-C6</f>
+        <f t="shared" si="0"/>
         <v>692.88999999999942</v>
       </c>
       <c r="E7" s="5">
-        <f>C7-$C$4</f>
+        <f t="shared" si="3"/>
         <v>2983.989999999998</v>
       </c>
       <c r="F7" s="4">
-        <f>+C7/C6-1</f>
+        <f t="shared" si="1"/>
         <v>1.3184785272711386E-2</v>
       </c>
       <c r="G7" s="7">
-        <f>C7/$C$4-1</f>
+        <f t="shared" si="2"/>
         <v>5.9369723806503405E-2</v>
       </c>
     </row>
@@ -1169,19 +1232,19 @@
         <v>53371.89</v>
       </c>
       <c r="D8" s="3">
-        <f>C8-C7</f>
+        <f t="shared" si="0"/>
         <v>126.76000000000204</v>
       </c>
       <c r="E8" s="5">
-        <f>C8-$C$4</f>
+        <f t="shared" si="3"/>
         <v>3110.75</v>
       </c>
       <c r="F8" s="4">
-        <f>+C8/C7-1</f>
+        <f t="shared" si="1"/>
         <v>2.3806872102669629E-3</v>
       </c>
       <c r="G8" s="7">
-        <f>C8/$C$4-1</f>
+        <f t="shared" si="2"/>
         <v>6.1891751758913482E-2</v>
       </c>
     </row>
@@ -1193,19 +1256,19 @@
         <v>53996.44</v>
       </c>
       <c r="D9" s="3">
-        <f>C9-C8</f>
+        <f t="shared" si="0"/>
         <v>624.55000000000291</v>
       </c>
       <c r="E9" s="5">
-        <f>C9-$C$4</f>
+        <f t="shared" si="3"/>
         <v>3735.3000000000029</v>
       </c>
       <c r="F9" s="4">
-        <f>+C9/C8-1</f>
+        <f t="shared" si="1"/>
         <v>1.1701852791797362E-2</v>
       </c>
       <c r="G9" s="7">
-        <f>C9/$C$4-1</f>
+        <f t="shared" si="2"/>
         <v>7.4317852718820188E-2</v>
       </c>
     </row>
@@ -1217,19 +1280,19 @@
         <v>53630.09</v>
       </c>
       <c r="D10" s="3">
-        <f>C10-C9</f>
+        <f t="shared" si="0"/>
         <v>-366.35000000000582</v>
       </c>
       <c r="E10" s="5">
-        <f>C10-$C$4</f>
+        <f t="shared" si="3"/>
         <v>3368.9499999999971</v>
       </c>
       <c r="F10" s="4">
-        <f>+C10/C9-1</f>
+        <f t="shared" si="1"/>
         <v>-6.7847065473206625E-3</v>
       </c>
       <c r="G10" s="7">
-        <f>C10/$C$4-1</f>
+        <f t="shared" si="2"/>
         <v>6.7028921349575388E-2</v>
       </c>
     </row>
@@ -1239,15 +1302,29 @@
         <v>44768</v>
       </c>
       <c r="C11" s="3">
-        <v>53927</v>
+        <v>52314.02</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="0"/>
+        <v>-1316.0699999999997</v>
       </c>
       <c r="E11" s="5">
-        <f>C11-$C$4</f>
-        <v>3665.8600000000006</v>
+        <f t="shared" si="3"/>
+        <v>2052.8799999999974</v>
+      </c>
+      <c r="F11" s="4">
+        <f t="shared" si="1"/>
+        <v>-2.4539768626157477E-2</v>
       </c>
       <c r="G11" s="7">
         <f>C11/$C$4-1</f>
-        <v>7.2936268457102216E-2</v>
+        <v>4.0844278502238485E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B12" s="1">
+        <f>+B11+1</f>
+        <v>44769</v>
       </c>
     </row>
   </sheetData>
@@ -1259,13 +1336,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{038FFE9E-7C90-4B6C-9246-D1FB4481747B}">
-  <dimension ref="B2:P188"/>
+  <dimension ref="B2:P215"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C165" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C183" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G189" sqref="G189"/>
+      <selection pane="bottomRight" activeCell="A216" sqref="A216"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -7195,6 +7272,865 @@
         <v>28</v>
       </c>
     </row>
+    <row r="190" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B190" t="s">
+        <v>16</v>
+      </c>
+      <c r="C190" t="s">
+        <v>201</v>
+      </c>
+      <c r="D190">
+        <v>100</v>
+      </c>
+      <c r="E190" s="6">
+        <v>14.585000000000001</v>
+      </c>
+      <c r="F190" s="6">
+        <v>14.03</v>
+      </c>
+      <c r="G190" s="6">
+        <v>-1458.5</v>
+      </c>
+      <c r="H190" s="6">
+        <v>-1</v>
+      </c>
+      <c r="I190" s="6">
+        <v>1459.5</v>
+      </c>
+      <c r="J190" s="6">
+        <v>0</v>
+      </c>
+      <c r="K190" s="6">
+        <v>-55.5</v>
+      </c>
+      <c r="L190" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="191" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B191" t="s">
+        <v>27</v>
+      </c>
+      <c r="D191">
+        <v>100</v>
+      </c>
+      <c r="E191" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G191" s="6">
+        <v>-1458.5</v>
+      </c>
+      <c r="H191" s="6">
+        <v>-1</v>
+      </c>
+      <c r="I191" s="6">
+        <v>1459.5</v>
+      </c>
+      <c r="J191" s="6">
+        <v>0</v>
+      </c>
+      <c r="K191" s="6">
+        <v>-55.5</v>
+      </c>
+    </row>
+    <row r="192" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B192" t="s">
+        <v>29</v>
+      </c>
+      <c r="C192" t="s">
+        <v>202</v>
+      </c>
+      <c r="D192">
+        <v>300</v>
+      </c>
+      <c r="E192" s="6">
+        <v>11.048</v>
+      </c>
+      <c r="F192" s="6">
+        <v>10.79</v>
+      </c>
+      <c r="G192" s="6">
+        <v>-3314.4</v>
+      </c>
+      <c r="H192" s="6">
+        <v>-1.5</v>
+      </c>
+      <c r="I192" s="6">
+        <v>3445.38</v>
+      </c>
+      <c r="J192" s="6">
+        <v>129.47999999999999</v>
+      </c>
+      <c r="K192" s="6">
+        <v>-77.400000000000006</v>
+      </c>
+      <c r="L192" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="193" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B193" t="s">
+        <v>31</v>
+      </c>
+      <c r="D193">
+        <v>300</v>
+      </c>
+      <c r="E193" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G193" s="6">
+        <v>-3314.4</v>
+      </c>
+      <c r="H193" s="6">
+        <v>-1.5</v>
+      </c>
+      <c r="I193" s="6">
+        <v>3445.38</v>
+      </c>
+      <c r="J193" s="6">
+        <v>129.47999999999999</v>
+      </c>
+      <c r="K193" s="6">
+        <v>-77.400000000000006</v>
+      </c>
+      <c r="L193" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="194" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B194" t="s">
+        <v>203</v>
+      </c>
+      <c r="C194" t="s">
+        <v>204</v>
+      </c>
+      <c r="D194">
+        <v>100</v>
+      </c>
+      <c r="E194" s="6">
+        <v>30.92</v>
+      </c>
+      <c r="F194" s="6">
+        <v>31.55</v>
+      </c>
+      <c r="G194" s="6">
+        <v>-3092</v>
+      </c>
+      <c r="H194" s="6">
+        <v>-1</v>
+      </c>
+      <c r="I194" s="6">
+        <v>3093</v>
+      </c>
+      <c r="J194" s="6">
+        <v>0</v>
+      </c>
+      <c r="K194" s="6">
+        <v>63</v>
+      </c>
+      <c r="L194" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="195" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B195" t="s">
+        <v>203</v>
+      </c>
+      <c r="C195" t="s">
+        <v>205</v>
+      </c>
+      <c r="D195">
+        <v>100</v>
+      </c>
+      <c r="E195" s="6">
+        <v>31.19</v>
+      </c>
+      <c r="F195" s="6">
+        <v>31.55</v>
+      </c>
+      <c r="G195" s="6">
+        <v>-3119</v>
+      </c>
+      <c r="H195" s="6">
+        <v>-1</v>
+      </c>
+      <c r="I195" s="6">
+        <v>3120</v>
+      </c>
+      <c r="J195" s="6">
+        <v>0</v>
+      </c>
+      <c r="K195" s="6">
+        <v>36</v>
+      </c>
+      <c r="L195" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="196" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B196" t="s">
+        <v>203</v>
+      </c>
+      <c r="C196" t="s">
+        <v>206</v>
+      </c>
+      <c r="D196">
+        <v>-50</v>
+      </c>
+      <c r="E196" s="6">
+        <v>31.251999999999999</v>
+      </c>
+      <c r="F196" s="6">
+        <v>31.55</v>
+      </c>
+      <c r="G196" s="6">
+        <v>1562.6</v>
+      </c>
+      <c r="H196" s="6">
+        <v>-1.04</v>
+      </c>
+      <c r="I196" s="6">
+        <v>-1546.5</v>
+      </c>
+      <c r="J196" s="6">
+        <v>15.06</v>
+      </c>
+      <c r="K196" s="6">
+        <v>-14.9</v>
+      </c>
+      <c r="L196" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="197" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B197" t="s">
+        <v>203</v>
+      </c>
+      <c r="C197" t="s">
+        <v>207</v>
+      </c>
+      <c r="D197">
+        <v>-150</v>
+      </c>
+      <c r="E197" s="6">
+        <v>31.215</v>
+      </c>
+      <c r="F197" s="6">
+        <v>31.55</v>
+      </c>
+      <c r="G197" s="6">
+        <v>4682.25</v>
+      </c>
+      <c r="H197" s="6">
+        <v>-1.1299999999999999</v>
+      </c>
+      <c r="I197" s="6">
+        <v>-4666.5</v>
+      </c>
+      <c r="J197" s="6">
+        <v>14.62</v>
+      </c>
+      <c r="K197" s="6">
+        <v>-50.25</v>
+      </c>
+      <c r="L197" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="198" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B198" t="s">
+        <v>208</v>
+      </c>
+      <c r="D198">
+        <v>0</v>
+      </c>
+      <c r="E198" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G198" s="6">
+        <v>33.85</v>
+      </c>
+      <c r="H198" s="6">
+        <v>-4.17</v>
+      </c>
+      <c r="I198" s="6">
+        <v>0</v>
+      </c>
+      <c r="J198" s="6">
+        <v>29.68</v>
+      </c>
+      <c r="K198" s="6">
+        <v>33.85</v>
+      </c>
+      <c r="L198" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="199" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B199" t="s">
+        <v>49</v>
+      </c>
+      <c r="C199" t="s">
+        <v>209</v>
+      </c>
+      <c r="D199">
+        <v>-100</v>
+      </c>
+      <c r="E199" s="6">
+        <v>15.9</v>
+      </c>
+      <c r="F199" s="6">
+        <v>17.43</v>
+      </c>
+      <c r="G199" s="6">
+        <v>1590</v>
+      </c>
+      <c r="H199" s="6">
+        <v>-1.05</v>
+      </c>
+      <c r="I199" s="6">
+        <v>-1588.95</v>
+      </c>
+      <c r="J199" s="6">
+        <v>0</v>
+      </c>
+      <c r="K199" s="6">
+        <v>-153</v>
+      </c>
+      <c r="L199" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="200" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B200" t="s">
+        <v>49</v>
+      </c>
+      <c r="C200" t="s">
+        <v>210</v>
+      </c>
+      <c r="D200">
+        <v>-100</v>
+      </c>
+      <c r="E200" s="6">
+        <v>16.309999999999999</v>
+      </c>
+      <c r="F200" s="6">
+        <v>17.43</v>
+      </c>
+      <c r="G200" s="6">
+        <v>1631</v>
+      </c>
+      <c r="H200" s="6">
+        <v>-1.05</v>
+      </c>
+      <c r="I200" s="6">
+        <v>-1629.95</v>
+      </c>
+      <c r="J200" s="6">
+        <v>0</v>
+      </c>
+      <c r="K200" s="6">
+        <v>-112</v>
+      </c>
+      <c r="L200" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="201" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B201" t="s">
+        <v>49</v>
+      </c>
+      <c r="C201" t="s">
+        <v>211</v>
+      </c>
+      <c r="D201">
+        <v>-100</v>
+      </c>
+      <c r="E201" s="6">
+        <v>16.579999999999998</v>
+      </c>
+      <c r="F201" s="6">
+        <v>17.43</v>
+      </c>
+      <c r="G201" s="6">
+        <v>1658</v>
+      </c>
+      <c r="H201" s="6">
+        <v>-1.05</v>
+      </c>
+      <c r="I201" s="6">
+        <v>-1656.95</v>
+      </c>
+      <c r="J201" s="6">
+        <v>0</v>
+      </c>
+      <c r="K201" s="6">
+        <v>-85</v>
+      </c>
+      <c r="L201" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="202" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B202" t="s">
+        <v>49</v>
+      </c>
+      <c r="C202" t="s">
+        <v>212</v>
+      </c>
+      <c r="D202">
+        <v>-100</v>
+      </c>
+      <c r="E202" s="6">
+        <v>17.5</v>
+      </c>
+      <c r="F202" s="6">
+        <v>17.43</v>
+      </c>
+      <c r="G202" s="6">
+        <v>1750</v>
+      </c>
+      <c r="H202" s="6">
+        <v>-1.05</v>
+      </c>
+      <c r="I202" s="6">
+        <v>-1748.95</v>
+      </c>
+      <c r="J202" s="6">
+        <v>0</v>
+      </c>
+      <c r="K202" s="6">
+        <v>7</v>
+      </c>
+      <c r="L202" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="203" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B203" t="s">
+        <v>51</v>
+      </c>
+      <c r="D203">
+        <v>-400</v>
+      </c>
+      <c r="E203" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G203" s="6">
+        <v>6629</v>
+      </c>
+      <c r="H203" s="6">
+        <v>-4.2</v>
+      </c>
+      <c r="I203" s="6">
+        <v>-6624.8</v>
+      </c>
+      <c r="J203" s="6">
+        <v>0</v>
+      </c>
+      <c r="K203" s="6">
+        <v>-343</v>
+      </c>
+      <c r="L203" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="204" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B204" t="s">
+        <v>68</v>
+      </c>
+      <c r="C204" t="s">
+        <v>213</v>
+      </c>
+      <c r="D204">
+        <v>-50</v>
+      </c>
+      <c r="E204" s="6">
+        <v>393.46</v>
+      </c>
+      <c r="F204" s="6">
+        <v>390.89</v>
+      </c>
+      <c r="G204" s="6">
+        <v>19673</v>
+      </c>
+      <c r="H204" s="6">
+        <v>-1.46</v>
+      </c>
+      <c r="I204" s="6">
+        <v>-19671.54</v>
+      </c>
+      <c r="J204" s="6">
+        <v>198.61</v>
+      </c>
+      <c r="K204" s="6">
+        <v>128.5</v>
+      </c>
+      <c r="L204" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="205" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B205" t="s">
+        <v>68</v>
+      </c>
+      <c r="C205" t="s">
+        <v>214</v>
+      </c>
+      <c r="D205">
+        <v>10</v>
+      </c>
+      <c r="E205" s="6">
+        <v>392.65</v>
+      </c>
+      <c r="F205" s="6">
+        <v>390.89</v>
+      </c>
+      <c r="G205" s="6">
+        <v>-3926.5</v>
+      </c>
+      <c r="H205" s="6">
+        <v>-1</v>
+      </c>
+      <c r="I205" s="6">
+        <v>3934.31</v>
+      </c>
+      <c r="J205" s="6">
+        <v>6.81</v>
+      </c>
+      <c r="K205" s="6">
+        <v>-17.600000000000001</v>
+      </c>
+      <c r="L205" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="206" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B206" t="s">
+        <v>68</v>
+      </c>
+      <c r="C206" t="s">
+        <v>215</v>
+      </c>
+      <c r="D206">
+        <v>10</v>
+      </c>
+      <c r="E206" s="6">
+        <v>392.61950000000002</v>
+      </c>
+      <c r="F206" s="6">
+        <v>390.89</v>
+      </c>
+      <c r="G206" s="6">
+        <v>-3926.2</v>
+      </c>
+      <c r="H206" s="6">
+        <v>-1</v>
+      </c>
+      <c r="I206" s="6">
+        <v>3934.31</v>
+      </c>
+      <c r="J206" s="6">
+        <v>7.11</v>
+      </c>
+      <c r="K206" s="6">
+        <v>-17.3</v>
+      </c>
+      <c r="L206" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="207" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B207" t="s">
+        <v>68</v>
+      </c>
+      <c r="C207" t="s">
+        <v>216</v>
+      </c>
+      <c r="D207">
+        <v>10</v>
+      </c>
+      <c r="E207" s="6">
+        <v>390.50619999999998</v>
+      </c>
+      <c r="F207" s="6">
+        <v>390.89</v>
+      </c>
+      <c r="G207" s="6">
+        <v>-3905.06</v>
+      </c>
+      <c r="H207" s="6">
+        <v>-1</v>
+      </c>
+      <c r="I207" s="6">
+        <v>3886.68</v>
+      </c>
+      <c r="J207" s="6">
+        <v>-19.38</v>
+      </c>
+      <c r="K207" s="6">
+        <v>3.84</v>
+      </c>
+      <c r="L207" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="208" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B208" t="s">
+        <v>68</v>
+      </c>
+      <c r="C208" t="s">
+        <v>217</v>
+      </c>
+      <c r="D208">
+        <v>20</v>
+      </c>
+      <c r="E208" s="6">
+        <v>390.96600000000001</v>
+      </c>
+      <c r="F208" s="6">
+        <v>390.89</v>
+      </c>
+      <c r="G208" s="6">
+        <v>-7819.32</v>
+      </c>
+      <c r="H208" s="6">
+        <v>-1</v>
+      </c>
+      <c r="I208" s="6">
+        <v>7717.64</v>
+      </c>
+      <c r="J208" s="6">
+        <v>-102.68</v>
+      </c>
+      <c r="K208" s="6">
+        <v>-1.52</v>
+      </c>
+      <c r="L208" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="209" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B209" t="s">
+        <v>79</v>
+      </c>
+      <c r="D209">
+        <v>0</v>
+      </c>
+      <c r="E209" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G209" s="6">
+        <v>95.92</v>
+      </c>
+      <c r="H209" s="6">
+        <v>-5.46</v>
+      </c>
+      <c r="I209" s="6">
+        <v>-198.61</v>
+      </c>
+      <c r="J209" s="6">
+        <v>90.47</v>
+      </c>
+      <c r="K209" s="6">
+        <v>95.92</v>
+      </c>
+      <c r="L209" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="210" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B210" t="s">
+        <v>155</v>
+      </c>
+      <c r="C210" t="s">
+        <v>218</v>
+      </c>
+      <c r="D210">
+        <v>100</v>
+      </c>
+      <c r="E210" s="6">
+        <v>39.08</v>
+      </c>
+      <c r="F210" s="6">
+        <v>39.340000000000003</v>
+      </c>
+      <c r="G210" s="6">
+        <v>-3908</v>
+      </c>
+      <c r="H210" s="6">
+        <v>-1</v>
+      </c>
+      <c r="I210" s="6">
+        <v>3902.33</v>
+      </c>
+      <c r="J210" s="6">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="K210" s="6">
+        <v>26</v>
+      </c>
+      <c r="L210" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="211" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B211" t="s">
+        <v>155</v>
+      </c>
+      <c r="C211" t="s">
+        <v>219</v>
+      </c>
+      <c r="D211">
+        <v>100</v>
+      </c>
+      <c r="E211" s="6">
+        <v>38.94</v>
+      </c>
+      <c r="F211" s="6">
+        <v>39.340000000000003</v>
+      </c>
+      <c r="G211" s="6">
+        <v>-3894</v>
+      </c>
+      <c r="H211" s="6">
+        <v>-1</v>
+      </c>
+      <c r="I211" s="6">
+        <v>3908.18</v>
+      </c>
+      <c r="J211" s="6">
+        <v>13.18</v>
+      </c>
+      <c r="K211" s="6">
+        <v>40</v>
+      </c>
+      <c r="L211" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="212" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B212" t="s">
+        <v>155</v>
+      </c>
+      <c r="C212" t="s">
+        <v>220</v>
+      </c>
+      <c r="D212">
+        <v>-100</v>
+      </c>
+      <c r="E212" s="6">
+        <v>39.340000000000003</v>
+      </c>
+      <c r="F212" s="6">
+        <v>39.340000000000003</v>
+      </c>
+      <c r="G212" s="6">
+        <v>3934</v>
+      </c>
+      <c r="H212" s="6">
+        <v>-1.1000000000000001</v>
+      </c>
+      <c r="I212" s="6">
+        <v>-3932.9</v>
+      </c>
+      <c r="J212" s="6">
+        <v>0</v>
+      </c>
+      <c r="K212" s="6">
+        <v>0</v>
+      </c>
+      <c r="L212" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="213" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B213" t="s">
+        <v>155</v>
+      </c>
+      <c r="C213" t="s">
+        <v>221</v>
+      </c>
+      <c r="D213">
+        <v>200</v>
+      </c>
+      <c r="E213" s="6">
+        <v>39.258000000000003</v>
+      </c>
+      <c r="F213" s="6">
+        <v>39.340000000000003</v>
+      </c>
+      <c r="G213" s="6">
+        <v>-7851.6</v>
+      </c>
+      <c r="H213" s="6">
+        <v>-1</v>
+      </c>
+      <c r="I213" s="6">
+        <v>7871.07</v>
+      </c>
+      <c r="J213" s="6">
+        <v>18.47</v>
+      </c>
+      <c r="K213" s="6">
+        <v>16.399999999999999</v>
+      </c>
+      <c r="L213" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="214" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B214" t="s">
+        <v>159</v>
+      </c>
+      <c r="D214">
+        <v>300</v>
+      </c>
+      <c r="E214" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G214" s="6">
+        <v>-11719.6</v>
+      </c>
+      <c r="H214" s="6">
+        <v>-4.0999999999999996</v>
+      </c>
+      <c r="I214" s="6">
+        <v>11748.69</v>
+      </c>
+      <c r="J214" s="6">
+        <v>33.950000000000003</v>
+      </c>
+      <c r="K214" s="6">
+        <v>82.4</v>
+      </c>
+      <c r="L214" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="215" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="B215" t="s">
+        <v>61</v>
+      </c>
+      <c r="G215" s="6">
+        <v>-9733.73</v>
+      </c>
+      <c r="H215">
+        <v>-20.43</v>
+      </c>
+      <c r="I215" s="6">
+        <v>9830.17</v>
+      </c>
+      <c r="J215" s="6">
+        <v>283.58</v>
+      </c>
+      <c r="K215" s="6">
+        <v>-263.73</v>
+      </c>
+      <c r="L215" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>